<commit_message>
Finished Week 6 Solutions
</commit_message>
<xml_diff>
--- a/Exercises/Week6/books.xlsx
+++ b/Exercises/Week6/books.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jducharme\Intro-to-Python\Exercises\Week6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1948379-011F-4AC8-B04A-4536E70CF885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BBA381-4B15-4A1C-9BD7-557CAD681EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FA3A0A39-E0A6-4D1F-9305-ECB52FE2E261}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FA3A0A39-E0A6-4D1F-9305-ECB52FE2E261}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -52,9 +52,6 @@
     <t>The Hobbit</t>
   </si>
   <si>
-    <t>J.R.R Tolkien</t>
-  </si>
-  <si>
     <t>Fantasy</t>
   </si>
   <si>
@@ -506,6 +503,9 @@
   </si>
   <si>
     <t>Daniel Defoe</t>
+  </si>
+  <si>
+    <t>J.R.R. Tolkien</t>
   </si>
 </sst>
 </file>
@@ -894,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3989544-E64D-4D02-AE0F-B3B604C6CDEB}">
   <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="F75" sqref="F75"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -918,7 +918,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -929,13 +929,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" s="1">
         <v>1937</v>
@@ -943,16 +943,16 @@
     </row>
     <row r="3" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1">
         <v>1997</v>
@@ -960,16 +960,16 @@
     </row>
     <row r="4" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" s="1">
         <v>1851</v>
@@ -977,16 +977,16 @@
     </row>
     <row r="5" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="1">
         <v>1864</v>
@@ -994,16 +994,16 @@
     </row>
     <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" s="1">
         <v>1844</v>
@@ -1011,16 +1011,16 @@
     </row>
     <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="1">
         <v>2012</v>
@@ -1028,16 +1028,16 @@
     </row>
     <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" s="1">
         <v>1977</v>
@@ -1045,16 +1045,16 @@
     </row>
     <row r="9" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" s="1">
         <v>1862</v>
@@ -1062,16 +1062,16 @@
     </row>
     <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10" s="1">
         <v>1950</v>
@@ -1079,16 +1079,16 @@
     </row>
     <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="D11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" s="1">
         <v>1949</v>
@@ -1096,16 +1096,16 @@
     </row>
     <row r="12" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" s="1">
         <v>1953</v>
@@ -1113,16 +1113,16 @@
     </row>
     <row r="13" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="C13" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E13" s="1">
         <v>1960</v>
@@ -1130,16 +1130,16 @@
     </row>
     <row r="14" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="D14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E14" s="1">
         <v>1951</v>
@@ -1147,16 +1147,16 @@
     </row>
     <row r="15" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E15" s="1">
         <v>1945</v>
@@ -1164,16 +1164,16 @@
     </row>
     <row r="16" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E16" s="1">
         <v>1954</v>
@@ -1181,16 +1181,16 @@
     </row>
     <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="E17" s="1">
         <v>1866</v>
@@ -1198,16 +1198,16 @@
     </row>
     <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="E18" s="1">
         <v>1605</v>
@@ -1215,16 +1215,16 @@
     </row>
     <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="D19" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E19" s="1">
         <v>1954</v>
@@ -1232,16 +1232,16 @@
     </row>
     <row r="20" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="D20" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E20" s="1">
         <v>1954</v>
@@ -1249,16 +1249,16 @@
     </row>
     <row r="21" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="D21" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E21" s="1">
         <v>1955</v>
@@ -1266,16 +1266,16 @@
     </row>
     <row r="22" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="D22" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E22" s="1">
         <v>1831</v>
@@ -1283,16 +1283,16 @@
     </row>
     <row r="23" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="D23" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E23" s="1">
         <v>1966</v>
@@ -1300,16 +1300,16 @@
     </row>
     <row r="24" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="D24" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E24" s="1">
         <v>1668</v>
@@ -1317,16 +1317,16 @@
     </row>
     <row r="25" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="D25" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E25" s="1">
         <v>1759</v>
@@ -1334,16 +1334,16 @@
     </row>
     <row r="26" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E26" s="1">
         <v>1868</v>
@@ -1351,16 +1351,16 @@
     </row>
     <row r="27" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="E27" s="1">
         <v>1848</v>
@@ -1368,16 +1368,16 @@
     </row>
     <row r="28" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="C28" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E28" s="1">
         <v>1897</v>
@@ -1385,16 +1385,16 @@
     </row>
     <row r="29" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="C29" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E29" s="1">
         <v>1597</v>
@@ -1402,16 +1402,16 @@
     </row>
     <row r="30" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E30" s="1">
         <v>1603</v>
@@ -1419,16 +1419,16 @@
     </row>
     <row r="31" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E31" s="1">
         <v>1599</v>
@@ -1436,16 +1436,16 @@
     </row>
     <row r="32" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="D32" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E32" s="1">
         <v>1923</v>
@@ -1453,16 +1453,16 @@
     </row>
     <row r="33" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="D33" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E33" s="1">
         <v>1916</v>
@@ -1470,16 +1470,16 @@
     </row>
     <row r="34" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="C34" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E34" s="1">
         <v>1845</v>
@@ -1487,16 +1487,16 @@
     </row>
     <row r="35" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E35" s="1">
         <v>1843</v>
@@ -1504,16 +1504,16 @@
     </row>
     <row r="36" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E36" s="1">
         <v>1846</v>
@@ -1521,16 +1521,16 @@
     </row>
     <row r="37" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="C37" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E37" s="1">
         <v>1859</v>
@@ -1538,16 +1538,16 @@
     </row>
     <row r="38" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="C38" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="E38" s="1">
         <v>1644</v>
@@ -1555,16 +1555,16 @@
     </row>
     <row r="39" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E39" s="1">
         <v>1687</v>
@@ -1572,16 +1572,16 @@
     </row>
     <row r="40" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="C40" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E40" s="1">
         <v>1892</v>
@@ -1589,16 +1589,16 @@
     </row>
     <row r="41" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="C41" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E41" s="1">
         <v>1813</v>
@@ -1606,16 +1606,16 @@
     </row>
     <row r="42" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E42" s="1">
         <v>1846</v>
@@ -1623,16 +1623,16 @@
     </row>
     <row r="43" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="C43" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E43" s="1">
         <v>2008</v>
@@ -1640,16 +1640,16 @@
     </row>
     <row r="44" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="C44" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E44" s="1">
         <v>2011</v>
@@ -1657,16 +1657,16 @@
     </row>
     <row r="45" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="C45" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E45" s="1">
         <v>2005</v>
@@ -1674,16 +1674,16 @@
     </row>
     <row r="46" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="E46" s="1">
         <v>2005</v>
@@ -1691,16 +1691,16 @@
     </row>
     <row r="47" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="C47" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E47" s="1">
         <v>1887</v>
@@ -1708,16 +1708,16 @@
     </row>
     <row r="48" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E48" s="1">
         <v>1902</v>
@@ -1725,16 +1725,16 @@
     </row>
     <row r="49" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E49" s="1">
         <v>1893</v>
@@ -1742,16 +1742,16 @@
     </row>
     <row r="50" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="C50" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E50" s="1">
         <v>1934</v>
@@ -1759,16 +1759,16 @@
     </row>
     <row r="51" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E51" s="1">
         <v>1937</v>
@@ -1776,16 +1776,16 @@
     </row>
     <row r="52" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="C52" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E52" s="1">
         <v>1985</v>
@@ -1793,16 +1793,16 @@
     </row>
     <row r="53" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="D53" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E53" s="1">
         <v>1943</v>
@@ -1810,16 +1810,16 @@
     </row>
     <row r="54" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="C54" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E54" s="1">
         <v>1668</v>
@@ -1827,16 +1827,16 @@
     </row>
     <row r="55" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="C55" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E55" s="1">
         <v>1886</v>
@@ -1844,16 +1844,16 @@
     </row>
     <row r="56" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="C56" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E56" s="1">
         <v>1930</v>
@@ -1861,16 +1861,16 @@
     </row>
     <row r="57" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="C57" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E57" s="1">
         <v>1996</v>
@@ -1878,16 +1878,16 @@
     </row>
     <row r="58" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="C58" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E58" s="1">
         <v>1955</v>
@@ -1895,16 +1895,16 @@
     </row>
     <row r="59" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E59" s="1">
         <v>1950</v>
@@ -1912,16 +1912,16 @@
     </row>
     <row r="60" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E60" s="1">
         <v>1952</v>
@@ -1929,16 +1929,16 @@
     </row>
     <row r="61" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E61" s="1">
         <v>1872</v>
@@ -1946,16 +1946,16 @@
     </row>
     <row r="62" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E62" s="1">
         <v>1875</v>
@@ -1963,16 +1963,16 @@
     </row>
     <row r="63" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>135</v>
-      </c>
       <c r="C63" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E63" s="1">
         <v>1925</v>
@@ -1980,16 +1980,16 @@
     </row>
     <row r="64" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>137</v>
-      </c>
       <c r="C64" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E64" s="1">
         <v>1850</v>
@@ -1997,16 +1997,16 @@
     </row>
     <row r="65" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="D65" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E65" s="1">
         <v>1977</v>
@@ -2014,16 +2014,16 @@
     </row>
     <row r="66" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="C66" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E66" s="1">
         <v>1993</v>
@@ -2031,16 +2031,16 @@
     </row>
     <row r="67" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="C67" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E67" s="1">
         <v>1818</v>
@@ -2048,16 +2048,16 @@
     </row>
     <row r="68" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>144</v>
-      </c>
       <c r="C68" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E68" s="1">
         <v>1871</v>
@@ -2065,16 +2065,16 @@
     </row>
     <row r="69" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="C69" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="D69" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E69" s="1">
         <v>1942</v>
@@ -2082,16 +2082,16 @@
     </row>
     <row r="70" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>149</v>
-      </c>
       <c r="C70" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E70" s="1">
         <v>1950</v>
@@ -2099,16 +2099,16 @@
     </row>
     <row r="71" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>151</v>
-      </c>
       <c r="C71" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E71" s="1">
         <v>1952</v>
@@ -2116,16 +2116,16 @@
     </row>
     <row r="72" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E72" s="1">
         <v>1869</v>
@@ -2133,16 +2133,16 @@
     </row>
     <row r="73" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>154</v>
-      </c>
       <c r="C73" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E73" s="1">
         <v>1883</v>
@@ -2150,16 +2150,16 @@
     </row>
     <row r="74" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B74" s="1" t="s">
-        <v>156</v>
-      </c>
       <c r="C74" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E74" s="1">
         <v>1719</v>

</xml_diff>